<commit_message>
Added census and geocode
</commit_message>
<xml_diff>
--- a/facilities.xlsx
+++ b/facilities.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/Workspace/Amitech/tdwi-accelerate-2017-python/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="680" windowWidth="28560" windowHeight="17380"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="179">
   <si>
     <t>price</t>
   </si>
@@ -556,23 +569,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -587,26 +602,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -894,20 +923,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,11 +965,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>700</v>
       </c>
       <c r="C2" t="s">
@@ -949,18 +984,18 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>750</v>
       </c>
       <c r="C3" t="s">
@@ -975,18 +1010,18 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>100</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>800</v>
       </c>
       <c r="C4" t="s">
@@ -1001,18 +1036,18 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>100</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>878</v>
       </c>
       <c r="C5" t="s">
@@ -1027,18 +1062,18 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>100</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>900</v>
       </c>
       <c r="C6" t="s">
@@ -1053,18 +1088,18 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>100</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>1000</v>
       </c>
       <c r="C7" t="s">
@@ -1079,18 +1114,18 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>100</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>1025</v>
       </c>
       <c r="C8" t="s">
@@ -1105,18 +1140,18 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>100</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>1026</v>
       </c>
       <c r="C9" t="s">
@@ -1131,18 +1166,18 @@
       <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>100</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>1124</v>
       </c>
       <c r="C10" t="s">
@@ -1157,18 +1192,18 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>100</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <v>1124</v>
       </c>
       <c r="C11" t="s">
@@ -1183,18 +1218,18 @@
       <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>100</v>
       </c>
       <c r="H11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>1500</v>
       </c>
       <c r="C12" t="s">
@@ -1209,18 +1244,18 @@
       <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>100</v>
       </c>
       <c r="H12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>1870</v>
       </c>
       <c r="C13" t="s">
@@ -1235,18 +1270,18 @@
       <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>100</v>
       </c>
       <c r="H13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>1900</v>
       </c>
       <c r="C14" t="s">
@@ -1261,18 +1296,18 @@
       <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>100</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>2165</v>
       </c>
       <c r="C15" t="s">
@@ -1287,18 +1322,18 @@
       <c r="F15" t="s">
         <v>10</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>100</v>
       </c>
       <c r="H15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>2595</v>
       </c>
       <c r="C16" t="s">
@@ -1313,18 +1348,18 @@
       <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>100</v>
       </c>
       <c r="H16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>2900</v>
       </c>
       <c r="C17" t="s">
@@ -1339,18 +1374,18 @@
       <c r="F17" t="s">
         <v>10</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>100</v>
       </c>
       <c r="H17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>2903</v>
       </c>
       <c r="C18" t="s">
@@ -1365,18 +1400,18 @@
       <c r="F18" t="s">
         <v>10</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>100</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>2936</v>
       </c>
       <c r="C19" t="s">
@@ -1391,18 +1426,18 @@
       <c r="F19" t="s">
         <v>10</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>100</v>
       </c>
       <c r="H19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>2936</v>
       </c>
       <c r="C20" t="s">
@@ -1417,18 +1452,18 @@
       <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>100</v>
       </c>
       <c r="H20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>2936</v>
       </c>
       <c r="C21" t="s">
@@ -1443,18 +1478,18 @@
       <c r="F21" t="s">
         <v>10</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>100</v>
       </c>
       <c r="H21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>2936</v>
       </c>
       <c r="C22" t="s">
@@ -1469,18 +1504,18 @@
       <c r="F22" t="s">
         <v>10</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>100</v>
       </c>
       <c r="H22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>3650</v>
       </c>
       <c r="C23" t="s">
@@ -1495,18 +1530,18 @@
       <c r="F23" t="s">
         <v>10</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23">
         <v>100</v>
       </c>
       <c r="H23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>4000</v>
       </c>
       <c r="C24" t="s">
@@ -1521,18 +1556,18 @@
       <c r="F24" t="s">
         <v>10</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>100</v>
       </c>
       <c r="H24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>5300</v>
       </c>
       <c r="C25" t="s">
@@ -1547,18 +1582,18 @@
       <c r="F25" t="s">
         <v>10</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>100</v>
       </c>
       <c r="H25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>5626</v>
       </c>
       <c r="C26" t="s">
@@ -1573,18 +1608,18 @@
       <c r="F26" t="s">
         <v>10</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>100</v>
       </c>
       <c r="H26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>5800</v>
       </c>
       <c r="C27" t="s">
@@ -1599,18 +1634,18 @@
       <c r="F27" t="s">
         <v>10</v>
       </c>
-      <c r="G27" t="n">
+      <c r="G27">
         <v>100</v>
       </c>
       <c r="H27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>6000</v>
       </c>
       <c r="C28" t="s">
@@ -1625,18 +1660,18 @@
       <c r="F28" t="s">
         <v>10</v>
       </c>
-      <c r="G28" t="n">
+      <c r="G28">
         <v>100</v>
       </c>
       <c r="H28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
@@ -1651,18 +1686,18 @@
       <c r="F29" t="s">
         <v>66</v>
       </c>
-      <c r="G29" t="n">
+      <c r="G29">
         <v>100</v>
       </c>
       <c r="H29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>1000</v>
       </c>
       <c r="C30" t="s">
@@ -1677,18 +1712,18 @@
       <c r="F30" t="s">
         <v>66</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G30">
         <v>100</v>
       </c>
       <c r="H30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>1050</v>
       </c>
       <c r="C31" t="s">
@@ -1703,18 +1738,18 @@
       <c r="F31" t="s">
         <v>66</v>
       </c>
-      <c r="G31" t="n">
+      <c r="G31">
         <v>100</v>
       </c>
       <c r="H31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>1139</v>
       </c>
       <c r="C32" t="s">
@@ -1729,18 +1764,18 @@
       <c r="F32" t="s">
         <v>66</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G32">
         <v>100</v>
       </c>
       <c r="H32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1" t="n">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>1307</v>
       </c>
       <c r="C33" t="s">
@@ -1755,18 +1790,18 @@
       <c r="F33" t="s">
         <v>66</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G33">
         <v>100</v>
       </c>
       <c r="H33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>1450</v>
       </c>
       <c r="C34" t="s">
@@ -1781,18 +1816,18 @@
       <c r="F34" t="s">
         <v>66</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34">
         <v>100</v>
       </c>
       <c r="H34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1" t="n">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>1500</v>
       </c>
       <c r="C35" t="s">
@@ -1807,18 +1842,18 @@
       <c r="F35" t="s">
         <v>66</v>
       </c>
-      <c r="G35" t="n">
+      <c r="G35">
         <v>100</v>
       </c>
       <c r="H35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1" t="n">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>2117</v>
       </c>
       <c r="C36" t="s">
@@ -1833,18 +1868,18 @@
       <c r="F36" t="s">
         <v>66</v>
       </c>
-      <c r="G36" t="n">
+      <c r="G36">
         <v>100</v>
       </c>
       <c r="H36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="1" t="n">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>2117</v>
       </c>
       <c r="C37" t="s">
@@ -1859,18 +1894,18 @@
       <c r="F37" t="s">
         <v>66</v>
       </c>
-      <c r="G37" t="n">
+      <c r="G37">
         <v>100</v>
       </c>
       <c r="H37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="1" t="n">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>2448</v>
       </c>
       <c r="C38" t="s">
@@ -1885,18 +1920,18 @@
       <c r="F38" t="s">
         <v>66</v>
       </c>
-      <c r="G38" t="n">
+      <c r="G38">
         <v>100</v>
       </c>
       <c r="H38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="1" t="n">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>2950</v>
       </c>
       <c r="C39" t="s">
@@ -1911,18 +1946,18 @@
       <c r="F39" t="s">
         <v>66</v>
       </c>
-      <c r="G39" t="n">
+      <c r="G39">
         <v>100</v>
       </c>
       <c r="H39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="1" t="n">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>3558</v>
       </c>
       <c r="C40" t="s">
@@ -1937,18 +1972,18 @@
       <c r="F40" t="s">
         <v>66</v>
       </c>
-      <c r="G40" t="n">
+      <c r="G40">
         <v>100</v>
       </c>
       <c r="H40" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="1" t="n">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>3716</v>
       </c>
       <c r="C41" t="s">
@@ -1963,18 +1998,18 @@
       <c r="F41" t="s">
         <v>66</v>
       </c>
-      <c r="G41" t="n">
+      <c r="G41">
         <v>100</v>
       </c>
       <c r="H41" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1" t="n">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>3981</v>
       </c>
       <c r="C42" t="s">
@@ -1989,18 +2024,18 @@
       <c r="F42" t="s">
         <v>66</v>
       </c>
-      <c r="G42" t="n">
+      <c r="G42">
         <v>100</v>
       </c>
       <c r="H42" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1" t="n">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" t="s">
@@ -2015,18 +2050,18 @@
       <c r="F43" t="s">
         <v>96</v>
       </c>
-      <c r="G43" t="n">
+      <c r="G43">
         <v>100</v>
       </c>
       <c r="H43" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="1" t="n">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" t="s">
@@ -2041,18 +2076,18 @@
       <c r="F44" t="s">
         <v>96</v>
       </c>
-      <c r="G44" t="n">
+      <c r="G44">
         <v>100</v>
       </c>
       <c r="H44" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1" t="n">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" t="s">
@@ -2067,18 +2102,18 @@
       <c r="F45" t="s">
         <v>96</v>
       </c>
-      <c r="G45" t="n">
+      <c r="G45">
         <v>100</v>
       </c>
       <c r="H45" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
@@ -2093,18 +2128,18 @@
       <c r="F46" t="s">
         <v>96</v>
       </c>
-      <c r="G46" t="n">
+      <c r="G46">
         <v>100</v>
       </c>
       <c r="H46" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
@@ -2119,18 +2154,18 @@
       <c r="F47" t="s">
         <v>96</v>
       </c>
-      <c r="G47" t="n">
+      <c r="G47">
         <v>100</v>
       </c>
       <c r="H47" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="1" t="n">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" t="s">
@@ -2145,18 +2180,18 @@
       <c r="F48" t="s">
         <v>96</v>
       </c>
-      <c r="G48" t="n">
+      <c r="G48">
         <v>100</v>
       </c>
       <c r="H48" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>0</v>
       </c>
       <c r="C49" t="s">
@@ -2171,18 +2206,18 @@
       <c r="F49" t="s">
         <v>96</v>
       </c>
-      <c r="G49" t="n">
+      <c r="G49">
         <v>100</v>
       </c>
       <c r="H49" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>500</v>
       </c>
       <c r="C50" t="s">
@@ -2197,18 +2232,18 @@
       <c r="F50" t="s">
         <v>96</v>
       </c>
-      <c r="G50" t="n">
+      <c r="G50">
         <v>100</v>
       </c>
       <c r="H50" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="1" t="n">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>600</v>
       </c>
       <c r="C51" t="s">
@@ -2223,18 +2258,18 @@
       <c r="F51" t="s">
         <v>96</v>
       </c>
-      <c r="G51" t="n">
+      <c r="G51">
         <v>100</v>
       </c>
       <c r="H51" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="1" t="n">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>600</v>
       </c>
       <c r="C52" t="s">
@@ -2249,18 +2284,18 @@
       <c r="F52" t="s">
         <v>96</v>
       </c>
-      <c r="G52" t="n">
+      <c r="G52">
         <v>100</v>
       </c>
       <c r="H52" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="1" t="n">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>600</v>
       </c>
       <c r="C53" t="s">
@@ -2275,18 +2310,18 @@
       <c r="F53" t="s">
         <v>96</v>
       </c>
-      <c r="G53" t="n">
+      <c r="G53">
         <v>100</v>
       </c>
       <c r="H53" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="1" t="n">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>650</v>
       </c>
       <c r="C54" t="s">
@@ -2301,18 +2336,18 @@
       <c r="F54" t="s">
         <v>96</v>
       </c>
-      <c r="G54" t="n">
+      <c r="G54">
         <v>100</v>
       </c>
       <c r="H54" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="1" t="n">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>781</v>
       </c>
       <c r="C55" t="s">
@@ -2327,18 +2362,18 @@
       <c r="F55" t="s">
         <v>96</v>
       </c>
-      <c r="G55" t="n">
+      <c r="G55">
         <v>100</v>
       </c>
       <c r="H55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="1" t="n">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>800</v>
       </c>
       <c r="C56" t="s">
@@ -2353,18 +2388,18 @@
       <c r="F56" t="s">
         <v>96</v>
       </c>
-      <c r="G56" t="n">
+      <c r="G56">
         <v>100</v>
       </c>
       <c r="H56" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="1" t="n">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>800</v>
       </c>
       <c r="C57" t="s">
@@ -2379,18 +2414,18 @@
       <c r="F57" t="s">
         <v>96</v>
       </c>
-      <c r="G57" t="n">
+      <c r="G57">
         <v>100</v>
       </c>
       <c r="H57" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="1" t="n">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>812</v>
       </c>
       <c r="C58" t="s">
@@ -2405,18 +2440,18 @@
       <c r="F58" t="s">
         <v>96</v>
       </c>
-      <c r="G58" t="n">
+      <c r="G58">
         <v>100</v>
       </c>
       <c r="H58" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="1" t="n">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>825</v>
       </c>
       <c r="C59" t="s">
@@ -2431,18 +2466,18 @@
       <c r="F59" t="s">
         <v>96</v>
       </c>
-      <c r="G59" t="n">
+      <c r="G59">
         <v>100</v>
       </c>
       <c r="H59" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="1" t="n">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>995</v>
       </c>
       <c r="C60" t="s">
@@ -2457,18 +2492,18 @@
       <c r="F60" t="s">
         <v>96</v>
       </c>
-      <c r="G60" t="n">
+      <c r="G60">
         <v>100</v>
       </c>
       <c r="H60" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="1" t="n">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>1050</v>
       </c>
       <c r="C61" t="s">
@@ -2483,18 +2518,18 @@
       <c r="F61" t="s">
         <v>96</v>
       </c>
-      <c r="G61" t="n">
+      <c r="G61">
         <v>100</v>
       </c>
       <c r="H61" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="1" t="n">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>1050</v>
       </c>
       <c r="C62" t="s">
@@ -2509,18 +2544,18 @@
       <c r="F62" t="s">
         <v>96</v>
       </c>
-      <c r="G62" t="n">
+      <c r="G62">
         <v>100</v>
       </c>
       <c r="H62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="1" t="n">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>1262</v>
       </c>
       <c r="C63" t="s">
@@ -2535,18 +2570,18 @@
       <c r="F63" t="s">
         <v>96</v>
       </c>
-      <c r="G63" t="n">
+      <c r="G63">
         <v>100</v>
       </c>
       <c r="H63" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="1" t="n">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>1500</v>
       </c>
       <c r="C64" t="s">
@@ -2561,18 +2596,18 @@
       <c r="F64" t="s">
         <v>96</v>
       </c>
-      <c r="G64" t="n">
+      <c r="G64">
         <v>100</v>
       </c>
       <c r="H64" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="1" t="n">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>3050</v>
       </c>
       <c r="C65" t="s">
@@ -2587,18 +2622,18 @@
       <c r="F65" t="s">
         <v>96</v>
       </c>
-      <c r="G65" t="n">
+      <c r="G65">
         <v>100</v>
       </c>
       <c r="H65" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="1" t="n">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>3449</v>
       </c>
       <c r="C66" t="s">
@@ -2613,18 +2648,18 @@
       <c r="F66" t="s">
         <v>96</v>
       </c>
-      <c r="G66" t="n">
+      <c r="G66">
         <v>100</v>
       </c>
       <c r="H66" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="1" t="n">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>3449</v>
       </c>
       <c r="C67" t="s">
@@ -2639,18 +2674,18 @@
       <c r="F67" t="s">
         <v>96</v>
       </c>
-      <c r="G67" t="n">
+      <c r="G67">
         <v>100</v>
       </c>
       <c r="H67" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="1" t="n">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>3480</v>
       </c>
       <c r="C68" t="s">
@@ -2665,18 +2700,18 @@
       <c r="F68" t="s">
         <v>96</v>
       </c>
-      <c r="G68" t="n">
+      <c r="G68">
         <v>100</v>
       </c>
       <c r="H68" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="1" t="n">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>4926</v>
       </c>
       <c r="C69" t="s">
@@ -2691,18 +2726,18 @@
       <c r="F69" t="s">
         <v>96</v>
       </c>
-      <c r="G69" t="n">
+      <c r="G69">
         <v>100</v>
       </c>
       <c r="H69" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="1" t="n">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>4926</v>
       </c>
       <c r="C70" t="s">
@@ -2717,18 +2752,18 @@
       <c r="F70" t="s">
         <v>96</v>
       </c>
-      <c r="G70" t="n">
+      <c r="G70">
         <v>100</v>
       </c>
       <c r="H70" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="1" t="n">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>1450</v>
       </c>
       <c r="C71" t="s">
@@ -2743,18 +2778,18 @@
       <c r="F71" t="s">
         <v>96</v>
       </c>
-      <c r="G71" t="n">
+      <c r="G71">
         <v>100</v>
       </c>
       <c r="H71" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="1" t="n">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>0</v>
       </c>
       <c r="C72" t="s">
@@ -2769,18 +2804,18 @@
       <c r="F72" t="s">
         <v>153</v>
       </c>
-      <c r="G72" t="n">
+      <c r="G72">
         <v>100</v>
       </c>
       <c r="H72" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="1" t="n">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
         <v>71</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>0</v>
       </c>
       <c r="C73" t="s">
@@ -2795,18 +2830,18 @@
       <c r="F73" t="s">
         <v>153</v>
       </c>
-      <c r="G73" t="n">
+      <c r="G73">
         <v>100</v>
       </c>
       <c r="H73" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="1" t="n">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>0</v>
       </c>
       <c r="C74" t="s">
@@ -2821,18 +2856,18 @@
       <c r="F74" t="s">
         <v>153</v>
       </c>
-      <c r="G74" t="n">
+      <c r="G74">
         <v>100</v>
       </c>
       <c r="H74" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="1" t="n">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>0</v>
       </c>
       <c r="C75" t="s">
@@ -2847,18 +2882,18 @@
       <c r="F75" t="s">
         <v>153</v>
       </c>
-      <c r="G75" t="n">
+      <c r="G75">
         <v>100</v>
       </c>
       <c r="H75" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="1" t="n">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>600</v>
       </c>
       <c r="C76" t="s">
@@ -2873,18 +2908,18 @@
       <c r="F76" t="s">
         <v>153</v>
       </c>
-      <c r="G76" t="n">
+      <c r="G76">
         <v>100</v>
       </c>
       <c r="H76" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="1" t="n">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>650</v>
       </c>
       <c r="C77" t="s">
@@ -2899,18 +2934,18 @@
       <c r="F77" t="s">
         <v>153</v>
       </c>
-      <c r="G77" t="n">
+      <c r="G77">
         <v>100</v>
       </c>
       <c r="H77" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="1" t="n">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>750</v>
       </c>
       <c r="C78" t="s">
@@ -2925,18 +2960,18 @@
       <c r="F78" t="s">
         <v>153</v>
       </c>
-      <c r="G78" t="n">
+      <c r="G78">
         <v>100</v>
       </c>
       <c r="H78" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="1" t="n">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>800</v>
       </c>
       <c r="C79" t="s">
@@ -2951,18 +2986,18 @@
       <c r="F79" t="s">
         <v>153</v>
       </c>
-      <c r="G79" t="n">
+      <c r="G79">
         <v>100</v>
       </c>
       <c r="H79" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="1" t="n">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>870</v>
       </c>
       <c r="C80" t="s">
@@ -2977,18 +3012,18 @@
       <c r="F80" t="s">
         <v>153</v>
       </c>
-      <c r="G80" t="n">
+      <c r="G80">
         <v>100</v>
       </c>
       <c r="H80" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="1" t="n">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>900</v>
       </c>
       <c r="C81" t="s">
@@ -3003,18 +3038,18 @@
       <c r="F81" t="s">
         <v>153</v>
       </c>
-      <c r="G81" t="n">
+      <c r="G81">
         <v>100</v>
       </c>
       <c r="H81" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="1" t="n">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>1200</v>
       </c>
       <c r="C82" t="s">
@@ -3029,18 +3064,18 @@
       <c r="F82" t="s">
         <v>153</v>
       </c>
-      <c r="G82" t="n">
+      <c r="G82">
         <v>100</v>
       </c>
       <c r="H82" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="1" t="n">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>1468</v>
       </c>
       <c r="C83" t="s">
@@ -3055,18 +3090,18 @@
       <c r="F83" t="s">
         <v>153</v>
       </c>
-      <c r="G83" t="n">
+      <c r="G83">
         <v>100</v>
       </c>
       <c r="H83" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="1" t="n">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>3214</v>
       </c>
       <c r="C84" t="s">
@@ -3081,7 +3116,7 @@
       <c r="F84" t="s">
         <v>153</v>
       </c>
-      <c r="G84" t="n">
+      <c r="G84">
         <v>100</v>
       </c>
       <c r="H84" t="s">
@@ -3089,6 +3124,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>